<commit_message>
Inclusão GrupoEmpresarial, Rendas e Balanco
</commit_message>
<xml_diff>
--- a/documentos/Gerador de código Pessoa.xlsx
+++ b/documentos/Gerador de código Pessoa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Implantacao\implantacaoSinqia\API\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Implantacao\implantacaoSinqia\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FAE2F8-E37A-40CC-ABD8-26D7FCF973C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAADB60A-3E86-4FB0-B9B7-EFF4AA7A3EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geração propriedades" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8383" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8608" uniqueCount="1218">
   <si>
     <t>tb_pes</t>
   </si>
@@ -3517,6 +3517,180 @@
   </si>
   <si>
     <t>verdade, tinha e</t>
+  </si>
+  <si>
+    <t>Código da Pessoa</t>
+  </si>
+  <si>
+    <t>Número da renda</t>
+  </si>
+  <si>
+    <t>Valor dos rendimentos</t>
+  </si>
+  <si>
+    <t>valRenda</t>
+  </si>
+  <si>
+    <t>Nome do empregador</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Tipo do logradouro</t>
+  </si>
+  <si>
+    <t>Logradouro do trabalho</t>
+  </si>
+  <si>
+    <t>logradouroTrabalho</t>
+  </si>
+  <si>
+    <t>complemento</t>
+  </si>
+  <si>
+    <t>Bairro do trabalho</t>
+  </si>
+  <si>
+    <t>bairroTrabalho</t>
+  </si>
+  <si>
+    <t>CEP do trabalho</t>
+  </si>
+  <si>
+    <t>cepTrabalho</t>
+  </si>
+  <si>
+    <t>Periodicidade da renda</t>
+  </si>
+  <si>
+    <t>Data validade da renda</t>
+  </si>
+  <si>
+    <t>dataValidadeRenda</t>
+  </si>
+  <si>
+    <t>Observação da renda</t>
+  </si>
+  <si>
+    <t>observacaoRenda</t>
+  </si>
+  <si>
+    <t>Data de atualização</t>
+  </si>
+  <si>
+    <t>Código do usuário da atualização</t>
+  </si>
+  <si>
+    <t>codigoUsuarioAtualizacao</t>
+  </si>
+  <si>
+    <t>Indicador situação</t>
+  </si>
+  <si>
+    <t>Tipo de renda</t>
+  </si>
+  <si>
+    <t>Código do município</t>
+  </si>
+  <si>
+    <t>Código do Índice</t>
+  </si>
+  <si>
+    <t>codigoIndice</t>
+  </si>
+  <si>
+    <t>Número do logradouro do empregador</t>
+  </si>
+  <si>
+    <t>numeroLogradouroEmpregador</t>
+  </si>
+  <si>
+    <t>Data de admissão</t>
+  </si>
+  <si>
+    <t>Data de demissão</t>
+  </si>
+  <si>
+    <t>DDD empregador</t>
+  </si>
+  <si>
+    <t>dddEmpregador</t>
+  </si>
+  <si>
+    <t>Telefone empregador</t>
+  </si>
+  <si>
+    <t>telefoneEmpregador</t>
+  </si>
+  <si>
+    <t>Ramal empregador</t>
+  </si>
+  <si>
+    <t>ramalEmpregador</t>
+  </si>
+  <si>
+    <t>CNPJ do empregador</t>
+  </si>
+  <si>
+    <t>cnpjEmpregador</t>
+  </si>
+  <si>
+    <t>Tipo de Empresa</t>
+  </si>
+  <si>
+    <t>tipoEmpresa</t>
+  </si>
+  <si>
+    <t>Identificador de renda conjugue</t>
+  </si>
+  <si>
+    <t>identificadorRendaConjugue</t>
+  </si>
+  <si>
+    <t>Identifica a renda corresp. empregador</t>
+  </si>
+  <si>
+    <t>identificaRendaCorrespEmpregador</t>
+  </si>
+  <si>
+    <t>Ano Balanço</t>
+  </si>
+  <si>
+    <t>anoBalanco</t>
+  </si>
+  <si>
+    <t>Sequencial Balanço</t>
+  </si>
+  <si>
+    <t>sequencialBalanco</t>
+  </si>
+  <si>
+    <t>Data início Balanço</t>
+  </si>
+  <si>
+    <t>dataInicioBalanco</t>
+  </si>
+  <si>
+    <t>Data fim Balanço</t>
+  </si>
+  <si>
+    <t>dataFimBalanco</t>
+  </si>
+  <si>
+    <t>Descrição Balanço</t>
+  </si>
+  <si>
+    <t>descricaoBalanco</t>
+  </si>
+  <si>
+    <t>Indicador de situação</t>
+  </si>
+  <si>
+    <t>Código do Detalhe – Linha Balanço</t>
+  </si>
+  <si>
+    <t>codigoDetalheLinhaBalanco</t>
   </si>
 </sst>
 </file>
@@ -3953,10 +4127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G387"/>
+  <dimension ref="A1:H435"/>
   <sheetViews>
-    <sheetView topLeftCell="D352" workbookViewId="0">
-      <selection activeCell="A363" sqref="A363"/>
+    <sheetView tabSelected="1" topLeftCell="D400" workbookViewId="0">
+      <selection activeCell="G421" sqref="G421:G435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12410,7 +12584,7 @@
         <v>|/// &lt;summary&gt;|/// Código ISPB do banco|/// &lt;/summary&gt;| public string codigoIspb { get; set; }</v>
       </c>
     </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385" s="20" t="s">
         <v>580</v>
       </c>
@@ -12432,7 +12606,7 @@
         <v>|/// &lt;summary&gt;|/// Código de Instituição de Pagamento|/// &lt;/summary&gt;| public decimal codigoInstPagamento { get; set; }</v>
       </c>
     </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386" s="20" t="s">
         <v>580</v>
       </c>
@@ -12454,8 +12628,968 @@
         <v>|/// &lt;summary&gt;|/// Indica se é Conta Padrão ou não - S - sim | N - não|/// &lt;/summary&gt;| public string indicadorContaPadrao { get; set; }</v>
       </c>
     </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387" s="18"/>
+      <c r="G387" s="18"/>
+      <c r="H387" s="18"/>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G388" s="18"/>
+      <c r="H388" s="18"/>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>411</v>
+      </c>
+      <c r="B389" t="s">
+        <v>1</v>
+      </c>
+      <c r="D389" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E389" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="F389" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G389" s="18" t="str">
+        <f t="shared" ref="G387:G435" si="6">CONCATENATE("|/// &lt;summary&gt;|/// ",D389,"|/// &lt;/summary&gt;| public ",F389," ",E389," { get; set; }")</f>
+        <v>|/// &lt;summary&gt;|/// Código da Pessoa|/// &lt;/summary&gt;| public string codigoPessoa { get; set; }</v>
+      </c>
+      <c r="H389" s="18"/>
+    </row>
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A390" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B390" t="s">
+        <v>412</v>
+      </c>
+      <c r="D390" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E390" s="19" t="s">
+        <v>982</v>
+      </c>
+      <c r="F390" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G390" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Número da renda|/// &lt;/summary&gt;| public int numeroRenda { get; set; }</v>
+      </c>
+      <c r="H390" s="18"/>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A391" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B391" t="s">
+        <v>414</v>
+      </c>
+      <c r="D391" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E391" s="19" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F391" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="G391" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Valor dos rendimentos|/// &lt;/summary&gt;| public decimal valRenda { get; set; }</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A392" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B392" t="s">
+        <v>416</v>
+      </c>
+      <c r="D392" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E392" s="19" t="s">
+        <v>818</v>
+      </c>
+      <c r="F392" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G392" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Nome do empregador|/// &lt;/summary&gt;| public string nomeEmpregador { get; set; }</v>
+      </c>
+    </row>
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A393" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B393" t="s">
+        <v>418</v>
+      </c>
+      <c r="D393" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E393" t="s">
+        <v>961</v>
+      </c>
+      <c r="F393" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G393" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Cargo|/// &lt;/summary&gt;| public string cargoEmpregador { get; set; }</v>
+      </c>
+    </row>
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A394" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B394" t="s">
+        <v>419</v>
+      </c>
+      <c r="D394" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E394" t="s">
+        <v>749</v>
+      </c>
+      <c r="F394" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G394" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Tipo do logradouro|/// &lt;/summary&gt;| public string tipoLogradouro { get; set; }</v>
+      </c>
+    </row>
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A395" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B395" t="s">
+        <v>420</v>
+      </c>
+      <c r="D395" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E395" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F395" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G395" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Logradouro do trabalho|/// &lt;/summary&gt;| public string logradouroTrabalho { get; set; }</v>
+      </c>
+    </row>
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A396" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B396" t="s">
+        <v>421</v>
+      </c>
+      <c r="D396" t="s">
+        <v>255</v>
+      </c>
+      <c r="E396" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F396" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G396" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Complemento|/// &lt;/summary&gt;| public string complemento { get; set; }</v>
+      </c>
+    </row>
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A397" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B397" t="s">
+        <v>422</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E397" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F397" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G397" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Bairro do trabalho|/// &lt;/summary&gt;| public string bairroTrabalho { get; set; }</v>
+      </c>
+    </row>
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A398" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B398" t="s">
+        <v>423</v>
+      </c>
+      <c r="D398" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E398" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F398" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G398" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// CEP do trabalho|/// &lt;/summary&gt;| public string cepTrabalho { get; set; }</v>
+      </c>
+    </row>
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A399" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B399" t="s">
+        <v>424</v>
+      </c>
+      <c r="D399" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E399" t="s">
+        <v>825</v>
+      </c>
+      <c r="F399" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G399" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Periodicidade da renda|/// &lt;/summary&gt;| public string periodicidadeRenda { get; set; }</v>
+      </c>
+    </row>
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A400" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B400" t="s">
+        <v>426</v>
+      </c>
+      <c r="D400" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E400" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F400" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G400" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data validade da renda|/// &lt;/summary&gt;| public DateTime dataValidadeRenda { get; set; }</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A401" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B401" t="s">
+        <v>428</v>
+      </c>
+      <c r="D401" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E401" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F401" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G401" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Observação da renda|/// &lt;/summary&gt;| public string observacaoRenda { get; set; }</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A402" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B402" t="s">
+        <v>26</v>
+      </c>
+      <c r="D402" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E402" t="s">
+        <v>642</v>
+      </c>
+      <c r="F402" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G402" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data de cadastramento|/// &lt;/summary&gt;| public DateTime dataCadastro { get; set; }</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A403" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B403" t="s">
+        <v>30</v>
+      </c>
+      <c r="D403" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E403" t="s">
+        <v>644</v>
+      </c>
+      <c r="F403" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G403" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data de atualização|/// &lt;/summary&gt;| public DateTime dataAtualizacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A404" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B404" t="s">
+        <v>28</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E404" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F404" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G404" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Código do usuário da atualização|/// &lt;/summary&gt;| public string codigoUsuarioAtualizacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A405" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B405" t="s">
+        <v>313</v>
+      </c>
+      <c r="D405" s="19" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E405" s="19" t="s">
+        <v>766</v>
+      </c>
+      <c r="F405" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G405" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Indicador situação|/// &lt;/summary&gt;| public string indicadorSituacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A406" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B406" t="s">
+        <v>139</v>
+      </c>
+      <c r="D406" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E406" t="s">
+        <v>767</v>
+      </c>
+      <c r="F406" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G406" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data da situação|/// &lt;/summary&gt;| public DateTime dataSituacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A407" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B407" t="s">
+        <v>429</v>
+      </c>
+      <c r="D407" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E407" t="s">
+        <v>824</v>
+      </c>
+      <c r="F407" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G407" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Tipo de renda|/// &lt;/summary&gt;| public int tipoRenda { get; set; }</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A408" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B408" t="s">
+        <v>38</v>
+      </c>
+      <c r="D408" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E408" t="s">
+        <v>648</v>
+      </c>
+      <c r="F408" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G408" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Código do município|/// &lt;/summary&gt;| public int codigoMunicipio { get; set; }</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A409" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B409" t="s">
+        <v>430</v>
+      </c>
+      <c r="D409" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E409" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F409" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G409" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Código do Índice|/// &lt;/summary&gt;| public string codigoIndice { get; set; }</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A410" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B410" t="s">
+        <v>432</v>
+      </c>
+      <c r="D410" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E410" s="18" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F410" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G410" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Número do logradouro do empregador|/// &lt;/summary&gt;| public string numeroLogradouroEmpregador { get; set; }</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A411" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B411" t="s">
+        <v>433</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E411" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="F411" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G411" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data de admissão|/// &lt;/summary&gt;| public DateTime dataAdmissao { get; set; }</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A412" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B412" t="s">
+        <v>435</v>
+      </c>
+      <c r="D412" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E412" t="s">
+        <v>829</v>
+      </c>
+      <c r="F412" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G412" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data de demissão|/// &lt;/summary&gt;| public DateTime dataDemissao { get; set; }</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A413" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B413" t="s">
+        <v>437</v>
+      </c>
+      <c r="D413" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E413" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F413" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G413" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// DDD empregador|/// &lt;/summary&gt;| public string dddEmpregador { get; set; }</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A414" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B414" t="s">
+        <v>438</v>
+      </c>
+      <c r="D414" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E414" s="18" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F414" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G414" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Telefone empregador|/// &lt;/summary&gt;| public string telefoneEmpregador { get; set; }</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A415" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B415" t="s">
+        <v>439</v>
+      </c>
+      <c r="D415" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E415" s="18" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F415" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G415" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Ramal empregador|/// &lt;/summary&gt;| public string ramalEmpregador { get; set; }</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A416" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B416" t="s">
+        <v>440</v>
+      </c>
+      <c r="D416" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E416" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F416" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G416" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// CNPJ do empregador|/// &lt;/summary&gt;| public string cnpjEmpregador { get; set; }</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A417" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B417" t="s">
+        <v>442</v>
+      </c>
+      <c r="D417" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E417" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F417" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G417" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Tipo de Empresa|/// &lt;/summary&gt;| public string tipoEmpresa { get; set; }</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A418" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B418" t="s">
+        <v>443</v>
+      </c>
+      <c r="D418" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E418" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F418" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G418" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Identificador de renda conjugue|/// &lt;/summary&gt;| public string identificadorRendaConjugue { get; set; }</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A419" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B419" t="s">
+        <v>445</v>
+      </c>
+      <c r="D419" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E419" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F419" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G419" s="18"/>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A420" s="18"/>
+      <c r="G420" s="18"/>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G421" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// |/// &lt;/summary&gt;| public   { get; set; }</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>482</v>
+      </c>
+      <c r="B422" t="s">
+        <v>1</v>
+      </c>
+      <c r="D422" t="s">
+        <v>245</v>
+      </c>
+      <c r="E422" s="18" t="s">
+        <v>630</v>
+      </c>
+      <c r="F422" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G422" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Código Pessoa|/// &lt;/summary&gt;| public string codigoPessoa { get; set; }</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>482</v>
+      </c>
+      <c r="B423" t="s">
+        <v>483</v>
+      </c>
+      <c r="D423" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E423" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F423" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G423" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Ano Balanço|/// &lt;/summary&gt;| public DateTime anoBalanco { get; set; }</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>482</v>
+      </c>
+      <c r="B424" t="s">
+        <v>485</v>
+      </c>
+      <c r="D424" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E424" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F424" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G424" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Sequencial Balanço|/// &lt;/summary&gt;| public int sequencialBalanco { get; set; }</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>482</v>
+      </c>
+      <c r="B425" t="s">
+        <v>487</v>
+      </c>
+      <c r="D425" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E425" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F425" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G425" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data início Balanço|/// &lt;/summary&gt;| public DateTime dataInicioBalanco { get; set; }</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>482</v>
+      </c>
+      <c r="B426" t="s">
+        <v>488</v>
+      </c>
+      <c r="D426" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E426" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F426" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G426" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data fim Balanço|/// &lt;/summary&gt;| public DateTime dataFimBalanco { get; set; }</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>482</v>
+      </c>
+      <c r="B427" t="s">
+        <v>489</v>
+      </c>
+      <c r="D427" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E427" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F427" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G427" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Descrição Balanço|/// &lt;/summary&gt;| public string descricaoBalanco { get; set; }</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>482</v>
+      </c>
+      <c r="B428" t="s">
+        <v>26</v>
+      </c>
+      <c r="D428" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E428" t="s">
+        <v>642</v>
+      </c>
+      <c r="F428" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G428" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data de cadastramento|/// &lt;/summary&gt;| public DateTime dataCadastro { get; set; }</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>482</v>
+      </c>
+      <c r="B429" t="s">
+        <v>28</v>
+      </c>
+      <c r="D429" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E429" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F429" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G429" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Código do usuário da atualização|/// &lt;/summary&gt;| public string codigoUsuarioAtualizacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>482</v>
+      </c>
+      <c r="B430" t="s">
+        <v>30</v>
+      </c>
+      <c r="D430" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E430" t="s">
+        <v>644</v>
+      </c>
+      <c r="F430" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G430" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data de atualização|/// &lt;/summary&gt;| public DateTime dataAtualizacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>482</v>
+      </c>
+      <c r="B431" t="s">
+        <v>313</v>
+      </c>
+      <c r="D431" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E431" t="s">
+        <v>766</v>
+      </c>
+      <c r="F431" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G431" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Indicador de situação|/// &lt;/summary&gt;| public string indicadorSituacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>482</v>
+      </c>
+      <c r="B432" t="s">
+        <v>139</v>
+      </c>
+      <c r="D432" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E432" t="s">
+        <v>767</v>
+      </c>
+      <c r="F432" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G432" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Data da situação|/// &lt;/summary&gt;| public DateTime dataSituacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>482</v>
+      </c>
+      <c r="B433" t="s">
+        <v>430</v>
+      </c>
+      <c r="D433" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E433" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F433" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G433" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Código do Índice|/// &lt;/summary&gt;| public string codigoIndice { get; set; }</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>482</v>
+      </c>
+      <c r="B434" t="s">
+        <v>490</v>
+      </c>
+      <c r="D434" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E434" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F434" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G434" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Código do Detalhe – Linha Balanço|/// &lt;/summary&gt;| public string codigoDetalheLinhaBalanco { get; set; }</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>482</v>
+      </c>
+      <c r="B435" t="s">
+        <v>492</v>
+      </c>
+      <c r="D435" t="s">
+        <v>493</v>
+      </c>
+      <c r="E435" t="s">
+        <v>857</v>
+      </c>
+      <c r="F435" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="G435" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>|/// &lt;summary&gt;|/// Valor Analisado|/// &lt;/summary&gt;| public decimal valorAnalisado { get; set; }</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12467,7 +13601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L359" workbookViewId="0">
+    <sheetView topLeftCell="A362" workbookViewId="0">
       <selection activeCell="M366" sqref="M366:M389"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Inserido adaptador de rendas
</commit_message>
<xml_diff>
--- a/documentos/Gerador de código Pessoa.xlsx
+++ b/documentos/Gerador de código Pessoa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Implantacao\implantacaoSinqia\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAADB60A-3E86-4FB0-B9B7-EFF4AA7A3EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A56AD-0D35-4599-8B96-E1C4E47320C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geração propriedades" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8608" uniqueCount="1218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8923" uniqueCount="1220">
   <si>
     <t>tb_pes</t>
   </si>
@@ -3691,6 +3691,12 @@
   </si>
   <si>
     <t>codigoDetalheLinhaBalanco</t>
+  </si>
+  <si>
+    <t>registroBalanco</t>
+  </si>
+  <si>
+    <t>registroRendas</t>
   </si>
 </sst>
 </file>
@@ -4129,8 +4135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D400" workbookViewId="0">
-      <selection activeCell="G421" sqref="G421:G435"/>
+    <sheetView topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="A389" sqref="A389:F419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12654,7 +12660,7 @@
         <v>3</v>
       </c>
       <c r="G389" s="18" t="str">
-        <f t="shared" ref="G387:G435" si="6">CONCATENATE("|/// &lt;summary&gt;|/// ",D389,"|/// &lt;/summary&gt;| public ",F389," ",E389," { get; set; }")</f>
+        <f t="shared" ref="G389:G435" si="6">CONCATENATE("|/// &lt;summary&gt;|/// ",D389,"|/// &lt;/summary&gt;| public ",F389," ",E389," { get; set; }")</f>
         <v>|/// &lt;summary&gt;|/// Código da Pessoa|/// &lt;/summary&gt;| public string codigoPessoa { get; set; }</v>
       </c>
       <c r="H389" s="18"/>
@@ -13599,10 +13605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M390"/>
+  <dimension ref="A1:M438"/>
   <sheetViews>
-    <sheetView topLeftCell="A362" workbookViewId="0">
-      <selection activeCell="M366" sqref="M366:M389"/>
+    <sheetView tabSelected="1" topLeftCell="A395" workbookViewId="0">
+      <selection activeCell="K406" sqref="K406:K407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29507,7 +29513,7 @@
         <v>1120</v>
       </c>
       <c r="I356" s="18" t="str">
-        <f t="shared" ref="I356:I389" si="30">CONCATENATE("public ",F356," ",B356,"  { get; set; }")</f>
+        <f t="shared" ref="I356:I405" si="30">CONCATENATE("public ",F356," ",B356,"  { get; set; }")</f>
         <v>public string cod_pessoa_assina1  { get; set; }</v>
       </c>
       <c r="J356" s="18" t="str">
@@ -30752,11 +30758,11 @@
         <v>public string NEGCODISPB  { get; set; }</v>
       </c>
       <c r="J387" s="18" t="str">
-        <f t="shared" ref="J387:J389" si="31">IF(F387="string",CONCATENATE("!string.IsNullOrWhiteSpace(",H387,".",E387,")"),IF(F387="int",CONCATENATE(H387,".",E387," != null &amp;&amp; ",H387,".",E387,".Value &gt; 0"),IF(F387="DateTime",CONCATENATE(H387,".",E387," != null &amp;&amp; ",H387,".",E387,".Value != DateTime.MinValue"),IF(F387="decimal",CONCATENATE(H387,".",E387," != null &amp;&amp; ",H387,".",E387,".Value &gt; 0")))))</f>
+        <f t="shared" ref="J387:J405" si="31">IF(F387="string",CONCATENATE("!string.IsNullOrWhiteSpace(",H387,".",E387,")"),IF(F387="int",CONCATENATE(H387,".",E387," != null &amp;&amp; ",H387,".",E387,".Value &gt; 0"),IF(F387="DateTime",CONCATENATE(H387,".",E387," != null &amp;&amp; ",H387,".",E387,".Value != DateTime.MinValue"),IF(F387="decimal",CONCATENATE(H387,".",E387," != null &amp;&amp; ",H387,".",E387,".Value &gt; 0")))))</f>
         <v>!string.IsNullOrWhiteSpace(msg.codigoIspb)</v>
       </c>
       <c r="K387" s="18" t="str">
-        <f t="shared" ref="K387:K389" si="32">CONCATENATE("|if(",J387,")","| ",G387,".",B387," = ",H387,".",E387,";")</f>
+        <f t="shared" ref="K387:K438" si="32">CONCATENATE("|if(",J387,")","| ",G387,".",B387," = ",H387,".",E387,";")</f>
         <v>|if(!string.IsNullOrWhiteSpace(msg.codigoIspb))| registroNegocio.NEGCODISPB = msg.codigoIspb;</v>
       </c>
       <c r="L387" s="18" t="str">
@@ -30858,6 +30864,1581 @@
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M390" s="19"/>
+    </row>
+    <row r="392" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A392" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B392" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D392" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E392" s="18" t="s">
+        <v>630</v>
+      </c>
+      <c r="F392" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G392" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H392" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I392" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public string cod_pessoa  { get; set; }</v>
+      </c>
+      <c r="J392" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>!string.IsNullOrWhiteSpace(msg.codigoPessoa)</v>
+      </c>
+      <c r="K392" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoa))| registroBalanco.cod_pessoa = msg.codigoPessoa;</v>
+      </c>
+    </row>
+    <row r="393" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A393" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B393" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="D393" s="18" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E393" s="18" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F393" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G393" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H393" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I393" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public DateTime ano_balanco  { get; set; }</v>
+      </c>
+      <c r="J393" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.anoBalanco != null &amp;&amp; msg.anoBalanco.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K393" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.anoBalanco != null &amp;&amp; msg.anoBalanco.Value != DateTime.MinValue)| registroBalanco.ano_balanco = msg.anoBalanco;</v>
+      </c>
+    </row>
+    <row r="394" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A394" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B394" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="D394" s="18" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E394" s="18" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F394" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G394" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H394" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I394" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public int seq_balanco  { get; set; }</v>
+      </c>
+      <c r="J394" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.sequencialBalanco != null &amp;&amp; msg.sequencialBalanco.Value &gt; 0</v>
+      </c>
+      <c r="K394" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.sequencialBalanco != null &amp;&amp; msg.sequencialBalanco.Value &gt; 0)| registroBalanco.seq_balanco = msg.sequencialBalanco;</v>
+      </c>
+    </row>
+    <row r="395" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A395" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B395" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="D395" s="18" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E395" s="18" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F395" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G395" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H395" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I395" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public DateTime dat_ini_balanco  { get; set; }</v>
+      </c>
+      <c r="J395" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.dataInicioBalanco != null &amp;&amp; msg.dataInicioBalanco.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K395" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataInicioBalanco != null &amp;&amp; msg.dataInicioBalanco.Value != DateTime.MinValue)| registroBalanco.dat_ini_balanco = msg.dataInicioBalanco;</v>
+      </c>
+    </row>
+    <row r="396" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A396" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B396" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="D396" s="18" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E396" s="18" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F396" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G396" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H396" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I396" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public DateTime dat_fim_balanco  { get; set; }</v>
+      </c>
+      <c r="J396" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.dataFimBalanco != null &amp;&amp; msg.dataFimBalanco.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K396" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataFimBalanco != null &amp;&amp; msg.dataFimBalanco.Value != DateTime.MinValue)| registroBalanco.dat_fim_balanco = msg.dataFimBalanco;</v>
+      </c>
+    </row>
+    <row r="397" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A397" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B397" s="18" t="s">
+        <v>489</v>
+      </c>
+      <c r="D397" s="18" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E397" s="18" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F397" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G397" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H397" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I397" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public string des_balanco  { get; set; }</v>
+      </c>
+      <c r="J397" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>!string.IsNullOrWhiteSpace(msg.descricaoBalanco)</v>
+      </c>
+      <c r="K397" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.descricaoBalanco))| registroBalanco.des_balanco = msg.descricaoBalanco;</v>
+      </c>
+    </row>
+    <row r="398" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A398" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B398" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D398" s="18" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E398" s="18" t="s">
+        <v>642</v>
+      </c>
+      <c r="F398" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G398" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H398" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I398" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public DateTime dat_cad  { get; set; }</v>
+      </c>
+      <c r="J398" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.dataCadastro != null &amp;&amp; msg.dataCadastro.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K398" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataCadastro != null &amp;&amp; msg.dataCadastro.Value != DateTime.MinValue)| registroBalanco.dat_cad = msg.dataCadastro;</v>
+      </c>
+    </row>
+    <row r="399" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A399" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B399" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D399" s="18" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E399" s="18" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F399" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G399" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H399" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I399" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public string usu_atu  { get; set; }</v>
+      </c>
+      <c r="J399" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>!string.IsNullOrWhiteSpace(msg.codigoUsuarioAtualizacao)</v>
+      </c>
+      <c r="K399" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoUsuarioAtualizacao))| registroBalanco.usu_atu = msg.codigoUsuarioAtualizacao;</v>
+      </c>
+    </row>
+    <row r="400" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A400" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B400" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D400" s="18" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E400" s="18" t="s">
+        <v>644</v>
+      </c>
+      <c r="F400" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G400" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H400" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I400" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public DateTime dat_atu  { get; set; }</v>
+      </c>
+      <c r="J400" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.dataAtualizacao != null &amp;&amp; msg.dataAtualizacao.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K400" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataAtualizacao != null &amp;&amp; msg.dataAtualizacao.Value != DateTime.MinValue)| registroBalanco.dat_atu = msg.dataAtualizacao;</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A401" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B401" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="D401" s="18" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E401" s="18" t="s">
+        <v>766</v>
+      </c>
+      <c r="F401" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G401" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H401" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I401" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public string idc_sit  { get; set; }</v>
+      </c>
+      <c r="J401" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>!string.IsNullOrWhiteSpace(msg.indicadorSituacao)</v>
+      </c>
+      <c r="K401" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorSituacao))| registroBalanco.idc_sit = msg.indicadorSituacao;</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A402" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B402" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D402" s="18" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E402" s="18" t="s">
+        <v>767</v>
+      </c>
+      <c r="F402" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G402" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H402" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I402" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public DateTime dat_sit  { get; set; }</v>
+      </c>
+      <c r="J402" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.dataSituacao != null &amp;&amp; msg.dataSituacao.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K402" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataSituacao != null &amp;&amp; msg.dataSituacao.Value != DateTime.MinValue)| registroBalanco.dat_sit = msg.dataSituacao;</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A403" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B403" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="D403" s="18" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E403" s="18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F403" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G403" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H403" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I403" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public string cod_ind  { get; set; }</v>
+      </c>
+      <c r="J403" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>!string.IsNullOrWhiteSpace(msg.codigoIndice)</v>
+      </c>
+      <c r="K403" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoIndice))| registroBalanco.cod_ind = msg.codigoIndice;</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A404" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B404" s="18" t="s">
+        <v>490</v>
+      </c>
+      <c r="D404" s="18" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E404" s="18" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F404" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G404" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H404" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I404" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public string cod_detalhe  { get; set; }</v>
+      </c>
+      <c r="J404" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>!string.IsNullOrWhiteSpace(msg.codigoDetalheLinhaBalanco)</v>
+      </c>
+      <c r="K404" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoDetalheLinhaBalanco))| registroBalanco.cod_detalhe = msg.codigoDetalheLinhaBalanco;</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A405" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B405" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="D405" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="E405" s="18" t="s">
+        <v>857</v>
+      </c>
+      <c r="F405" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="G405" s="19" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H405" s="19" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I405" s="18" t="str">
+        <f t="shared" si="30"/>
+        <v>public decimal val_analisado  { get; set; }</v>
+      </c>
+      <c r="J405" s="18" t="str">
+        <f t="shared" si="31"/>
+        <v>msg.valorAnalisado != null &amp;&amp; msg.valorAnalisado.Value &gt; 0</v>
+      </c>
+      <c r="K405" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.valorAnalisado != null &amp;&amp; msg.valorAnalisado.Value &gt; 0)| registroBalanco.val_analisado = msg.valorAnalisado;</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A408" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B408" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D408" s="18" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E408" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="F408" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G408" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H408" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I408" s="18" t="str">
+        <f t="shared" ref="I406:I438" si="35">CONCATENATE("public ",F408," ",B408,"  { get; set; }")</f>
+        <v>public string cod_pessoa  { get; set; }</v>
+      </c>
+      <c r="J408" s="18" t="str">
+        <f t="shared" ref="J406:J438" si="36">IF(F408="string",CONCATENATE("!string.IsNullOrWhiteSpace(",H408,".",E408,")"),IF(F408="int",CONCATENATE(H408,".",E408," != null &amp;&amp; ",H408,".",E408,".Value &gt; 0"),IF(F408="DateTime",CONCATENATE(H408,".",E408," != null &amp;&amp; ",H408,".",E408,".Value != DateTime.MinValue"),IF(F408="decimal",CONCATENATE(H408,".",E408," != null &amp;&amp; ",H408,".",E408,".Value &gt; 0")))))</f>
+        <v>!string.IsNullOrWhiteSpace(msg.codigoPessoa)</v>
+      </c>
+      <c r="K408" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoa))| registroRendas.cod_pessoa = msg.codigoPessoa;</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A409" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B409" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="D409" s="18" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E409" s="19" t="s">
+        <v>982</v>
+      </c>
+      <c r="F409" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G409" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H409" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I409" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public int num_renda  { get; set; }</v>
+      </c>
+      <c r="J409" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.numeroRenda != null &amp;&amp; msg.numeroRenda.Value &gt; 0</v>
+      </c>
+      <c r="K409" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.numeroRenda != null &amp;&amp; msg.numeroRenda.Value &gt; 0)| registroRendas.num_renda = msg.numeroRenda;</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A410" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B410" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="D410" s="18" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E410" s="19" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F410" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="G410" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H410" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I410" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public decimal val_renda  { get; set; }</v>
+      </c>
+      <c r="J410" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.valRenda != null &amp;&amp; msg.valRenda.Value &gt; 0</v>
+      </c>
+      <c r="K410" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.valRenda != null &amp;&amp; msg.valRenda.Value &gt; 0)| registroRendas.val_renda = msg.valRenda;</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A411" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B411" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="D411" s="18" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E411" s="19" t="s">
+        <v>818</v>
+      </c>
+      <c r="F411" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G411" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H411" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I411" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string nom_empreg  { get; set; }</v>
+      </c>
+      <c r="J411" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.nomeEmpregador)</v>
+      </c>
+      <c r="K411" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeEmpregador))| registroRendas.nom_empreg = msg.nomeEmpregador;</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A412" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B412" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="D412" s="18" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E412" s="18" t="s">
+        <v>961</v>
+      </c>
+      <c r="F412" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G412" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H412" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I412" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string crg_empreg  { get; set; }</v>
+      </c>
+      <c r="J412" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.cargoEmpregador)</v>
+      </c>
+      <c r="K412" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.cargoEmpregador))| registroRendas.crg_empreg = msg.cargoEmpregador;</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A413" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B413" s="18" t="s">
+        <v>419</v>
+      </c>
+      <c r="D413" s="18" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E413" s="18" t="s">
+        <v>749</v>
+      </c>
+      <c r="F413" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G413" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H413" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I413" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string tip_log_empreg  { get; set; }</v>
+      </c>
+      <c r="J413" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.tipoLogradouro)</v>
+      </c>
+      <c r="K413" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoLogradouro))| registroRendas.tip_log_empreg = msg.tipoLogradouro;</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A414" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B414" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="D414" s="18" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E414" s="18" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F414" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G414" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H414" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I414" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string end_empreg  { get; set; }</v>
+      </c>
+      <c r="J414" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.logradouroTrabalho)</v>
+      </c>
+      <c r="K414" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.logradouroTrabalho))| registroRendas.end_empreg = msg.logradouroTrabalho;</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A415" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B415" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="D415" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E415" s="18" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F415" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G415" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H415" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I415" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string cpl_log_empreg  { get; set; }</v>
+      </c>
+      <c r="J415" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.complemento)</v>
+      </c>
+      <c r="K415" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.complemento))| registroRendas.cpl_log_empreg = msg.complemento;</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A416" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B416" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="D416" s="19" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E416" s="18" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F416" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G416" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H416" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I416" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string bai_empreg  { get; set; }</v>
+      </c>
+      <c r="J416" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.bairroTrabalho)</v>
+      </c>
+      <c r="K416" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.bairroTrabalho))| registroRendas.bai_empreg = msg.bairroTrabalho;</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A417" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B417" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="D417" s="18" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E417" s="18" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F417" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G417" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H417" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I417" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string cep_empreg  { get; set; }</v>
+      </c>
+      <c r="J417" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.cepTrabalho)</v>
+      </c>
+      <c r="K417" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.cepTrabalho))| registroRendas.cep_empreg = msg.cepTrabalho;</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A418" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B418" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="D418" s="18" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E418" s="18" t="s">
+        <v>825</v>
+      </c>
+      <c r="F418" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G418" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H418" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I418" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string per_renda  { get; set; }</v>
+      </c>
+      <c r="J418" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.periodicidadeRenda)</v>
+      </c>
+      <c r="K418" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.periodicidadeRenda))| registroRendas.per_renda = msg.periodicidadeRenda;</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A419" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B419" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="D419" s="18" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E419" s="18" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F419" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G419" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H419" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I419" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public DateTime dat_vld_renda  { get; set; }</v>
+      </c>
+      <c r="J419" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.dataValidadeRenda != null &amp;&amp; msg.dataValidadeRenda.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K419" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataValidadeRenda != null &amp;&amp; msg.dataValidadeRenda.Value != DateTime.MinValue)| registroRendas.dat_vld_renda = msg.dataValidadeRenda;</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A420" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B420" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="D420" s="18" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E420" s="18" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F420" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G420" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H420" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I420" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string obs_renda  { get; set; }</v>
+      </c>
+      <c r="J420" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.observacaoRenda)</v>
+      </c>
+      <c r="K420" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.observacaoRenda))| registroRendas.obs_renda = msg.observacaoRenda;</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A421" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B421" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D421" s="18" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E421" s="18" t="s">
+        <v>642</v>
+      </c>
+      <c r="F421" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G421" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H421" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I421" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public DateTime dat_cad  { get; set; }</v>
+      </c>
+      <c r="J421" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.dataCadastro != null &amp;&amp; msg.dataCadastro.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K421" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataCadastro != null &amp;&amp; msg.dataCadastro.Value != DateTime.MinValue)| registroRendas.dat_cad = msg.dataCadastro;</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A422" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B422" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D422" s="18" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E422" s="18" t="s">
+        <v>644</v>
+      </c>
+      <c r="F422" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G422" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H422" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I422" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public DateTime dat_atu  { get; set; }</v>
+      </c>
+      <c r="J422" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.dataAtualizacao != null &amp;&amp; msg.dataAtualizacao.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K422" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataAtualizacao != null &amp;&amp; msg.dataAtualizacao.Value != DateTime.MinValue)| registroRendas.dat_atu = msg.dataAtualizacao;</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A423" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B423" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D423" s="19" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E423" s="18" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F423" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G423" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H423" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I423" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string usu_atu  { get; set; }</v>
+      </c>
+      <c r="J423" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.codigoUsuarioAtualizacao)</v>
+      </c>
+      <c r="K423" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoUsuarioAtualizacao))| registroRendas.usu_atu = msg.codigoUsuarioAtualizacao;</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A424" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B424" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="D424" s="19" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E424" s="19" t="s">
+        <v>766</v>
+      </c>
+      <c r="F424" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G424" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H424" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I424" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string idc_sit  { get; set; }</v>
+      </c>
+      <c r="J424" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.indicadorSituacao)</v>
+      </c>
+      <c r="K424" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorSituacao))| registroRendas.idc_sit = msg.indicadorSituacao;</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A425" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B425" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D425" s="18" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E425" s="18" t="s">
+        <v>767</v>
+      </c>
+      <c r="F425" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G425" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H425" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I425" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public DateTime dat_sit  { get; set; }</v>
+      </c>
+      <c r="J425" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.dataSituacao != null &amp;&amp; msg.dataSituacao.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K425" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataSituacao != null &amp;&amp; msg.dataSituacao.Value != DateTime.MinValue)| registroRendas.dat_sit = msg.dataSituacao;</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A426" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B426" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="D426" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E426" s="18" t="s">
+        <v>824</v>
+      </c>
+      <c r="F426" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G426" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H426" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I426" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public int tip_renda  { get; set; }</v>
+      </c>
+      <c r="J426" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.tipoRenda != null &amp;&amp; msg.tipoRenda.Value &gt; 0</v>
+      </c>
+      <c r="K426" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.tipoRenda != null &amp;&amp; msg.tipoRenda.Value &gt; 0)| registroRendas.tip_renda = msg.tipoRenda;</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A427" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B427" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D427" s="18" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E427" s="18" t="s">
+        <v>648</v>
+      </c>
+      <c r="F427" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="G427" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H427" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I427" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public int cod_municipio  { get; set; }</v>
+      </c>
+      <c r="J427" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.codigoMunicipio != null &amp;&amp; msg.codigoMunicipio.Value &gt; 0</v>
+      </c>
+      <c r="K427" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.codigoMunicipio != null &amp;&amp; msg.codigoMunicipio.Value &gt; 0)| registroRendas.cod_municipio = msg.codigoMunicipio;</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A428" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B428" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="D428" s="18" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E428" s="18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F428" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G428" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H428" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I428" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string cod_ind  { get; set; }</v>
+      </c>
+      <c r="J428" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.codigoIndice)</v>
+      </c>
+      <c r="K428" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoIndice))| registroRendas.cod_ind = msg.codigoIndice;</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A429" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B429" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="D429" s="18" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E429" s="18" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F429" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G429" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H429" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I429" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string num_log_empreg  { get; set; }</v>
+      </c>
+      <c r="J429" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.numeroLogradouroEmpregador)</v>
+      </c>
+      <c r="K429" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroLogradouroEmpregador))| registroRendas.num_log_empreg = msg.numeroLogradouroEmpregador;</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A430" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B430" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="D430" s="19" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E430" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="F430" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G430" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H430" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I430" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public DateTime dat_admissao  { get; set; }</v>
+      </c>
+      <c r="J430" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.dataAdmissao != null &amp;&amp; msg.dataAdmissao.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K430" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataAdmissao != null &amp;&amp; msg.dataAdmissao.Value != DateTime.MinValue)| registroRendas.dat_admissao = msg.dataAdmissao;</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A431" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B431" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="D431" s="18" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E431" s="18" t="s">
+        <v>829</v>
+      </c>
+      <c r="F431" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G431" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H431" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I431" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public DateTime dat_demissao  { get; set; }</v>
+      </c>
+      <c r="J431" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>msg.dataDemissao != null &amp;&amp; msg.dataDemissao.Value != DateTime.MinValue</v>
+      </c>
+      <c r="K431" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(msg.dataDemissao != null &amp;&amp; msg.dataDemissao.Value != DateTime.MinValue)| registroRendas.dat_demissao = msg.dataDemissao;</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A432" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B432" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="D432" s="18" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E432" s="18" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F432" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G432" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H432" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I432" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string ddd_empreg  { get; set; }</v>
+      </c>
+      <c r="J432" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.dddEmpregador)</v>
+      </c>
+      <c r="K432" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.dddEmpregador))| registroRendas.ddd_empreg = msg.dddEmpregador;</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A433" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B433" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="D433" s="18" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E433" s="18" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F433" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G433" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H433" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I433" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string tel_empreg  { get; set; }</v>
+      </c>
+      <c r="J433" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.telefoneEmpregador)</v>
+      </c>
+      <c r="K433" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.telefoneEmpregador))| registroRendas.tel_empreg = msg.telefoneEmpregador;</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A434" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B434" s="18" t="s">
+        <v>439</v>
+      </c>
+      <c r="D434" s="18" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E434" s="18" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F434" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G434" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H434" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I434" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string ram_empreg  { get; set; }</v>
+      </c>
+      <c r="J434" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.ramalEmpregador)</v>
+      </c>
+      <c r="K434" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.ramalEmpregador))| registroRendas.ram_empreg = msg.ramalEmpregador;</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A435" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B435" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="D435" s="18" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E435" s="18" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F435" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G435" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H435" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I435" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string cod_cnpj  { get; set; }</v>
+      </c>
+      <c r="J435" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.cnpjEmpregador)</v>
+      </c>
+      <c r="K435" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.cnpjEmpregador))| registroRendas.cod_cnpj = msg.cnpjEmpregador;</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A436" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B436" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="D436" s="18" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E436" s="18" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F436" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G436" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H436" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I436" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string tip_emp  { get; set; }</v>
+      </c>
+      <c r="J436" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.tipoEmpresa)</v>
+      </c>
+      <c r="K436" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoEmpresa))| registroRendas.tip_emp = msg.tipoEmpresa;</v>
+      </c>
+    </row>
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A437" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B437" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="D437" s="18" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E437" s="18" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F437" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G437" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H437" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I437" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string renidtrencon  { get; set; }</v>
+      </c>
+      <c r="J437" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.identificadorRendaConjugue)</v>
+      </c>
+      <c r="K437" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.identificadorRendaConjugue))| registroRendas.renidtrencon = msg.identificadorRendaConjugue;</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A438" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B438" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="D438" s="18" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E438" s="18" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F438" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G438" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H438" s="18" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I438" s="18" t="str">
+        <f t="shared" si="35"/>
+        <v>public string renidtemp  { get; set; }</v>
+      </c>
+      <c r="J438" s="18" t="str">
+        <f t="shared" si="36"/>
+        <v>!string.IsNullOrWhiteSpace(msg.identificaRendaCorrespEmpregador)</v>
+      </c>
+      <c r="K438" s="18" t="str">
+        <f t="shared" si="32"/>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.identificaRendaCorrespEmpregador))| registroRendas.renidtemp = msg.identificaRendaCorrespEmpregador;</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>